<commit_message>
reviewed and edited for kill switch module for desktop
</commit_message>
<xml_diff>
--- a/test_case_report/sprint_38.xlsx
+++ b/test_case_report/sprint_38.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\test_case_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8311DFF-E331-4521-A75C-49F780363E30}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC478242-567C-4A8B-98CD-99527B78E791}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,19 +713,25 @@
       <c r="B37" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="1"/>
+      <c r="C37" s="1">
+        <v>579</v>
+      </c>
     </row>
     <row r="38" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="2"/>
+      <c r="C38" s="2">
+        <v>824</v>
+      </c>
     </row>
     <row r="39" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="3"/>
+      <c r="C39" s="3">
+        <v>615</v>
+      </c>
     </row>
     <row r="42" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
@@ -737,19 +743,25 @@
       <c r="B43" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="1"/>
+      <c r="C43" s="1">
+        <v>629</v>
+      </c>
     </row>
     <row r="44" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C44" s="2"/>
+      <c r="C44" s="2">
+        <v>854</v>
+      </c>
     </row>
     <row r="45" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C45" s="3"/>
+      <c r="C45" s="3">
+        <v>615</v>
+      </c>
     </row>
     <row r="48" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">

</xml_diff>